<commit_message>
set up for call from python
</commit_message>
<xml_diff>
--- a/server/test/inlet_test.xlsx
+++ b/server/test/inlet_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hailey.johnson\Documents\models\GEE\webApp\cem-utility\server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hailey.johnson\Documents\models\GEE\webApp\cem-utility\server\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,170 +336,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ26"/>
+  <dimension ref="A1:AZ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Y30" sqref="Y30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-      <c r="J1">
-        <v>0</v>
-      </c>
-      <c r="K1">
-        <v>0</v>
-      </c>
-      <c r="L1">
-        <v>0</v>
-      </c>
-      <c r="M1">
-        <v>0</v>
-      </c>
-      <c r="N1">
-        <v>0</v>
-      </c>
-      <c r="O1">
-        <v>0</v>
-      </c>
-      <c r="P1">
-        <v>0</v>
-      </c>
-      <c r="Q1">
-        <v>0</v>
-      </c>
-      <c r="R1">
-        <v>0</v>
-      </c>
-      <c r="S1">
-        <v>0</v>
-      </c>
-      <c r="T1">
-        <v>0</v>
-      </c>
-      <c r="U1">
-        <v>0</v>
-      </c>
-      <c r="V1">
-        <v>0</v>
-      </c>
-      <c r="W1">
-        <v>0</v>
-      </c>
-      <c r="X1">
-        <v>0</v>
-      </c>
-      <c r="Y1">
-        <v>0</v>
-      </c>
-      <c r="Z1">
-        <v>0</v>
-      </c>
-      <c r="AA1">
-        <v>0</v>
-      </c>
-      <c r="AB1">
-        <v>0</v>
-      </c>
-      <c r="AC1">
-        <v>0</v>
-      </c>
-      <c r="AD1">
-        <v>0</v>
-      </c>
-      <c r="AE1">
-        <v>0</v>
-      </c>
-      <c r="AF1">
-        <v>0</v>
-      </c>
-      <c r="AG1">
-        <v>0</v>
-      </c>
-      <c r="AH1">
-        <v>0</v>
-      </c>
-      <c r="AI1">
-        <v>0</v>
-      </c>
-      <c r="AJ1">
-        <v>0</v>
-      </c>
-      <c r="AK1">
-        <v>0</v>
-      </c>
-      <c r="AL1">
-        <v>0</v>
-      </c>
-      <c r="AM1">
-        <v>0</v>
-      </c>
-      <c r="AN1">
-        <v>0</v>
-      </c>
-      <c r="AO1">
-        <v>0</v>
-      </c>
-      <c r="AP1">
-        <v>0</v>
-      </c>
-      <c r="AQ1">
-        <v>0</v>
-      </c>
-      <c r="AR1">
-        <v>0</v>
-      </c>
-      <c r="AS1">
-        <v>0</v>
-      </c>
-      <c r="AT1">
-        <v>0</v>
-      </c>
-      <c r="AU1">
-        <v>0</v>
-      </c>
-      <c r="AV1">
-        <v>0</v>
-      </c>
-      <c r="AW1">
-        <v>0</v>
-      </c>
-      <c r="AX1">
-        <v>0</v>
-      </c>
-      <c r="AY1">
-        <v>0</v>
-      </c>
-      <c r="AZ1">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
@@ -1140,28 +986,28 @@
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1322,28 +1168,28 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1504,7 +1350,7 @@
         <v>1</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -1522,94 +1368,94 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
@@ -1650,10 +1496,10 @@
         <v>1</v>
       </c>
       <c r="M9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <v>1</v>
@@ -1677,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="V9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9">
         <v>1</v>
@@ -1820,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -1835,7 +1681,7 @@
         <v>0</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10">
         <v>1</v>
@@ -1930,52 +1776,52 @@
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -1996,94 +1842,94 @@
         <v>0</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
@@ -2121,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -2130,7 +1976,7 @@
         <v>1</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -2282,10 +2128,10 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -3668,160 +3514,160 @@
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.25">
@@ -4453,6 +4299,164 @@
         <v>1</v>
       </c>
       <c r="AZ26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="X27">
+        <v>1</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AB27">
+        <v>1</v>
+      </c>
+      <c r="AC27">
+        <v>1</v>
+      </c>
+      <c r="AD27">
+        <v>1</v>
+      </c>
+      <c r="AE27">
+        <v>1</v>
+      </c>
+      <c r="AF27">
+        <v>1</v>
+      </c>
+      <c r="AG27">
+        <v>1</v>
+      </c>
+      <c r="AH27">
+        <v>1</v>
+      </c>
+      <c r="AI27">
+        <v>1</v>
+      </c>
+      <c r="AJ27">
+        <v>1</v>
+      </c>
+      <c r="AK27">
+        <v>1</v>
+      </c>
+      <c r="AL27">
+        <v>1</v>
+      </c>
+      <c r="AM27">
+        <v>1</v>
+      </c>
+      <c r="AN27">
+        <v>1</v>
+      </c>
+      <c r="AO27">
+        <v>1</v>
+      </c>
+      <c r="AP27">
+        <v>1</v>
+      </c>
+      <c r="AQ27">
+        <v>1</v>
+      </c>
+      <c r="AR27">
+        <v>1</v>
+      </c>
+      <c r="AS27">
+        <v>1</v>
+      </c>
+      <c r="AT27">
+        <v>1</v>
+      </c>
+      <c r="AU27">
+        <v>1</v>
+      </c>
+      <c r="AV27">
+        <v>1</v>
+      </c>
+      <c r="AW27">
+        <v>1</v>
+      </c>
+      <c r="AX27">
+        <v>1</v>
+      </c>
+      <c r="AY27">
+        <v>1</v>
+      </c>
+      <c r="AZ27">
         <v>1</v>
       </c>
     </row>

</xml_diff>